<commit_message>
&& - №100021230 от 28.09.2024 www.coins-market.ru - №71214195 от 28.09.2024 https://meshok.net/ - №71036376 от 22.09.2024 https://meshok.net/ - №71214186 от 28.09.2024 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Germany/#EURO#Germany#Commemorative#[2006-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Germany/#EURO#Germany#Commemorative#[2006-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Germany\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1397CF-0EF8-46EC-9719-5A2BB2EC90A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50ABCE46-ED2F-4353-961C-61CD84245190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7970" yWindow="1450" windowWidth="28720" windowHeight="19550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -1568,7 +1568,7 @@
       <pane xSplit="17" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="R1" sqref="R1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P11" sqref="N11:P11"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1795,7 +1795,7 @@
         <v>32</v>
       </c>
       <c r="K5" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="7">
         <v>1</v>
@@ -1948,7 +1948,7 @@
         <v>44</v>
       </c>
       <c r="K8" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="7">
         <v>1</v>
@@ -2167,10 +2167,10 @@
         <v>1</v>
       </c>
       <c r="N12" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" s="17" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
& - №78318617 от 10.05.2025 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Germany/#EURO#Germany#Commemorative#[2006-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Germany/#EURO#Germany#Commemorative#[2006-present]#UNC%varieties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Germany\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9654C353-4E0F-4708-96FF-C345DE659734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AABDDD-41CC-4896-9BC8-B4642F209071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="207">
   <si>
     <t>Year</t>
   </si>
@@ -821,6 +821,9 @@
   </si>
   <si>
     <t>4.316.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          </t>
   </si>
 </sst>
 </file>
@@ -1187,14 +1190,15 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="16">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BE5FF"/>
-          <bgColor rgb="FF9BE5FF"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1211,23 +1215,6 @@
           <bgColor rgb="FF9BE5FF"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BE5FF"/>
-          <bgColor rgb="FF9BE5FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1338,9 +1325,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="5" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1615,7 +1602,7 @@
       <pane xSplit="17" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="R1" sqref="R1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomRight" activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3393,19 +3380,19 @@
         <v>203</v>
       </c>
       <c r="K35" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O35" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" s="17" t="str">
         <f t="shared" ref="P35:P36" si="4">IF(OR(AND(K35&gt;1,K35&lt;&gt;"-"),AND(L35&gt;1,L35&lt;&gt;"-"),AND(M35&gt;1,M35&lt;&gt;"-"),AND(N35&gt;1,N35&lt;&gt;"-"),AND(O35&gt;1,O35&lt;&gt;"-")),"Can exchange","")</f>
@@ -3452,6 +3439,9 @@
       <c r="Q36" s="25"/>
     </row>
     <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P37" s="8" t="s">
+        <v>206</v>
+      </c>
       <c r="Q37" s="25"/>
     </row>
   </sheetData>
@@ -3463,7 +3453,7 @@
     <mergeCell ref="K1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:O6 K8:O26">
-    <cfRule type="containsText" dxfId="17" priority="35" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="15" priority="35" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="36">
@@ -3478,7 +3468,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:O27">
-    <cfRule type="containsText" dxfId="16" priority="33" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="14" priority="33" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K27))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="34">
@@ -3493,7 +3483,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:O28 K30:O30 K32:O32">
-    <cfRule type="containsText" dxfId="15" priority="31" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="13" priority="31" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K28))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="32">
@@ -3508,7 +3498,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29:O29 K31:O31">
-    <cfRule type="containsText" dxfId="14" priority="29" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="12" priority="29" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K29))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="30">
@@ -3523,7 +3513,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:O34">
-    <cfRule type="containsText" dxfId="13" priority="27" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="11" priority="27" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K34))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="28">
@@ -3538,7 +3528,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:O33">
-    <cfRule type="containsText" dxfId="12" priority="25" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="10" priority="25" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K33))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="26">
@@ -3553,7 +3543,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="11" priority="23" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="9" priority="23" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K7))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="24">
@@ -3568,7 +3558,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="containsText" dxfId="10" priority="21" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="8" priority="21" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(L7))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="22">
@@ -3583,7 +3573,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(O7))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -3598,7 +3588,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(M7))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="12">
@@ -3613,7 +3603,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(N7))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -3628,7 +3618,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:O35">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K35))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -3643,7 +3633,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:O36">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K36))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">

</xml_diff>